<commit_message>
schematic update and gerber updates with corrections
</commit_message>
<xml_diff>
--- a/bom/ELIESTER_V2.xlsx
+++ b/bom/ELIESTER_V2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\eliester_esp32_printer\eliester_v2\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{91D73F93-7C32-47A5-A3BA-4B04E5088BDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B8EE94FC-D3A0-4B7C-B58A-6033F14FB56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ELIESTER_V2" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="640" uniqueCount="384">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="665" uniqueCount="394">
   <si>
     <t>Qty</t>
   </si>
@@ -567,9 +567,6 @@
     <t>R72</t>
   </si>
   <si>
-    <t>100K</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -807,9 +804,6 @@
     <t>C55, C59, C91</t>
   </si>
   <si>
-    <t>C57, C58, C87, C88, C89</t>
-  </si>
-  <si>
     <t>D1, D11</t>
   </si>
   <si>
@@ -837,9 +831,6 @@
     <t>L9, L10, L11</t>
   </si>
   <si>
-    <t>Q1, Q2, Q11, Q12</t>
-  </si>
-  <si>
     <t>Q3, Q4, Q6</t>
   </si>
   <si>
@@ -894,12 +885,6 @@
     <t>R70, R71, R73</t>
   </si>
   <si>
-    <t>R74, R76, R78</t>
-  </si>
-  <si>
-    <t>R75, R77</t>
-  </si>
-  <si>
     <t>SW2, SW3</t>
   </si>
   <si>
@@ -1119,9 +1104,6 @@
     <t>0402WGF220JTCE</t>
   </si>
   <si>
-    <t>0603WAF1003T5E</t>
-  </si>
-  <si>
     <t>0603WAF4701T5E</t>
   </si>
   <si>
@@ -1173,17 +1155,65 @@
     <t>XYCEELNANF-12.000000MHZ</t>
   </si>
   <si>
-    <t>S3225000161060C3</t>
-  </si>
-  <si>
     <t>LCSC</t>
+  </si>
+  <si>
+    <t>TZ1669D</t>
+  </si>
+  <si>
+    <t>C57,C58</t>
+  </si>
+  <si>
+    <t>C87, C88, C89</t>
+  </si>
+  <si>
+    <t>16p</t>
+  </si>
+  <si>
+    <t>7M25000013</t>
+  </si>
+  <si>
+    <t>Q9,Q10</t>
+  </si>
+  <si>
+    <t>2N7002</t>
+  </si>
+  <si>
+    <t>R74,R75,R67,R68</t>
+  </si>
+  <si>
+    <t>R76,R69</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> R78</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Fuse:Fuse_1210_3225Metric_Pad1.42x2.65mm_HandSolder</t>
+  </si>
+  <si>
+    <t>JK30-250</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>greencharge-footprints:fuse-JK30-200</t>
+  </si>
+  <si>
+    <t>SL1210190</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1314,6 +1344,20 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1622,7 +1666,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1665,12 +1709,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1704,6 +1750,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2023,11 +2070,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F128"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2054,7 +2101,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>
@@ -2062,7 +2109,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -2071,10 +2118,10 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="E2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -2091,10 +2138,10 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E3" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -2102,7 +2149,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -2111,10 +2158,10 @@
         <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E4" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -2122,7 +2169,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -2131,10 +2178,10 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E5" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -2142,7 +2189,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -2151,10 +2198,10 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E6" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F6">
         <v>16</v>
@@ -2162,7 +2209,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -2171,10 +2218,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E7" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F7">
         <v>6</v>
@@ -2182,7 +2229,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
@@ -2191,10 +2238,10 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E8" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F8">
         <v>7</v>
@@ -2202,7 +2249,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
@@ -2211,10 +2258,10 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E9" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -2222,7 +2269,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -2231,10 +2278,10 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E10" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -2251,10 +2298,10 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="E11" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -2262,7 +2309,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B12" t="s">
         <v>20</v>
@@ -2271,10 +2318,10 @@
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E12" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -2282,7 +2329,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
@@ -2291,10 +2338,10 @@
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E13" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -2311,10 +2358,10 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E14" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -2331,10 +2378,10 @@
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E15" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -2342,7 +2389,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
@@ -2351,10 +2398,10 @@
         <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E16" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F16">
         <v>4</v>
@@ -2362,7 +2409,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B17" t="s">
         <v>25</v>
@@ -2371,10 +2418,10 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="E17" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F17">
         <v>3</v>
@@ -2382,7 +2429,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
@@ -2391,10 +2438,10 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="E18" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F18">
         <v>3</v>
@@ -2411,10 +2458,10 @@
         <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="E19" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2431,10 +2478,10 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E20" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2451,10 +2498,10 @@
         <v>13</v>
       </c>
       <c r="D21" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E21" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2462,7 +2509,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
@@ -2471,10 +2518,10 @@
         <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E22" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F22">
         <v>3</v>
@@ -2491,10 +2538,10 @@
         <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E23" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -2502,7 +2549,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B24" t="s">
         <v>34</v>
@@ -2511,10 +2558,10 @@
         <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="E24" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -2531,10 +2578,10 @@
         <v>13</v>
       </c>
       <c r="D25" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="E25" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2542,7 +2589,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B26" t="s">
         <v>37</v>
@@ -2551,10 +2598,10 @@
         <v>13</v>
       </c>
       <c r="D26" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E26" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F26">
         <v>2</v>
@@ -2562,7 +2609,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B27" t="s">
         <v>23</v>
@@ -2571,10 +2618,10 @@
         <v>13</v>
       </c>
       <c r="D27" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E27" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -2594,7 +2641,7 @@
         <v>41</v>
       </c>
       <c r="E28" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2602,7 +2649,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>260</v>
+        <v>379</v>
       </c>
       <c r="B29" t="s">
         <v>42</v>
@@ -2611,50 +2658,50 @@
         <v>13</v>
       </c>
       <c r="D29" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E29" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>378</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>380</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>317</v>
+        <v>13</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>381</v>
       </c>
       <c r="E30" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C31" t="s">
         <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="E31" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F31">
         <v>1</v>
@@ -2662,19 +2709,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="E32" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -2682,19 +2729,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="C33" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>314</v>
       </c>
       <c r="E33" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -2702,19 +2749,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="D34" t="s">
-        <v>320</v>
+        <v>51</v>
       </c>
       <c r="E34" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -2722,19 +2769,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
         <v>13</v>
       </c>
       <c r="D35" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E35" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -2742,119 +2789,119 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>261</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="D36" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="E36" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>259</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="E37" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>262</v>
+        <v>58</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" t="s">
         <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E38" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F38">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>260</v>
       </c>
       <c r="B39" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C39" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>320</v>
       </c>
       <c r="E39" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>263</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E40" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F40">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D41" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E41" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -2862,19 +2909,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D42" t="s">
         <v>69</v>
       </c>
       <c r="E42" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F42">
         <v>2</v>
@@ -2882,19 +2929,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F43">
         <v>2</v>
@@ -2902,39 +2949,39 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>264</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E44" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D45" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="E45" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2942,19 +2989,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C46" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E46" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2962,19 +3009,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="D47" t="s">
-        <v>323</v>
+        <v>77</v>
       </c>
       <c r="E47" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2982,19 +3029,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B48" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C48" t="s">
         <v>57</v>
       </c>
       <c r="D48" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="E48" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -3002,19 +3049,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C49" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="D49" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="E49" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -3022,19 +3069,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D50" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="E50" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -3042,19 +3089,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C51" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D51" t="s">
-        <v>92</v>
+        <v>322</v>
       </c>
       <c r="E51" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -3062,59 +3109,59 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>267</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D52" t="s">
-        <v>329</v>
+        <v>92</v>
       </c>
       <c r="E52" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F52">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>265</v>
       </c>
       <c r="B53" t="s">
         <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D53" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E53" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B54" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C54" t="s">
-        <v>99</v>
-      </c>
-      <c r="D54">
-        <v>1050170001</v>
+        <v>96</v>
+      </c>
+      <c r="D54" t="s">
+        <v>325</v>
       </c>
       <c r="E54" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -3122,19 +3169,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B55" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
-      </c>
-      <c r="D55" t="s">
-        <v>331</v>
+        <v>99</v>
+      </c>
+      <c r="D55">
+        <v>1050170001</v>
       </c>
       <c r="E55" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -3142,19 +3189,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C56" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D56" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E56" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -3162,59 +3209,59 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>268</v>
+        <v>103</v>
       </c>
       <c r="B57" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C57" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D57" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="E57" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F57">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>266</v>
       </c>
       <c r="B58" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C58" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D58" t="s">
-        <v>109</v>
+        <v>328</v>
       </c>
       <c r="E58" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C59" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D59" t="s">
-        <v>333</v>
+        <v>109</v>
       </c>
       <c r="E59" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -3222,19 +3269,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B60" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C60" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D60" t="s">
-        <v>114</v>
+        <v>328</v>
       </c>
       <c r="E60" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -3242,59 +3289,59 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>269</v>
+        <v>113</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C61" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D61" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E61" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F61">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>118</v>
+        <v>267</v>
       </c>
       <c r="B62" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C62" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D62" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E62" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B63" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C63" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D63" t="s">
-        <v>334</v>
+        <v>121</v>
       </c>
       <c r="E63" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -3302,19 +3349,19 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B64" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C64" t="s">
         <v>124</v>
       </c>
       <c r="D64" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="E64" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -3322,99 +3369,99 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>270</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C65" t="s">
-        <v>64</v>
+        <v>124</v>
       </c>
       <c r="D65" t="s">
-        <v>127</v>
+        <v>330</v>
       </c>
       <c r="E65" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F65">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>271</v>
+        <v>386</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C66" t="s">
         <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E66" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F66">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>268</v>
       </c>
       <c r="B67" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C67" t="s">
         <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E67" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>272</v>
+        <v>129</v>
       </c>
       <c r="B68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C68" t="s">
         <v>64</v>
       </c>
       <c r="D68" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E68" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F68">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C69" t="s">
-        <v>133</v>
+        <v>64</v>
       </c>
       <c r="D69" t="s">
-        <v>336</v>
+        <v>131</v>
       </c>
       <c r="E69" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F69">
         <v>2</v>
@@ -3422,19 +3469,19 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B70" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C70" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D70" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="E70" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F70">
         <v>2</v>
@@ -3442,19 +3489,19 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C71" t="s">
         <v>135</v>
       </c>
       <c r="D71" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E71" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F71">
         <v>2</v>
@@ -3462,67 +3509,67 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C72" t="s">
         <v>135</v>
       </c>
       <c r="D72" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="E72" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F72">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C73" t="s">
         <v>135</v>
       </c>
       <c r="D73" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="E73" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F73">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>139</v>
+        <v>274</v>
       </c>
       <c r="B74" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C74" t="s">
         <v>135</v>
       </c>
       <c r="D74" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E74" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F74">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>278</v>
+        <v>139</v>
       </c>
       <c r="B75" t="s">
         <v>140</v>
@@ -3531,130 +3578,130 @@
         <v>135</v>
       </c>
       <c r="D75" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E75" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F75">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>141</v>
+        <v>275</v>
       </c>
       <c r="B76" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C76" t="s">
         <v>135</v>
       </c>
       <c r="D76" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="E76" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>279</v>
+        <v>141</v>
       </c>
       <c r="B77" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C77" t="s">
         <v>135</v>
       </c>
       <c r="D77" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="E77" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F77">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C78" t="s">
         <v>135</v>
       </c>
       <c r="D78" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="E78" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F78">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B79" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C79" t="s">
         <v>135</v>
       </c>
       <c r="D79" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="E79" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F79">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>146</v>
+        <v>278</v>
       </c>
       <c r="B80" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C80" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D80" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="E80" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F80">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B81" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C81" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D81" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="E81" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -3662,19 +3709,19 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B82" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C82" t="s">
         <v>135</v>
       </c>
       <c r="D82" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E82" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -3682,19 +3729,19 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B83" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C83" t="s">
         <v>135</v>
       </c>
       <c r="D83" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E83" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -3702,19 +3749,19 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B84" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="C84" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D84" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="E84" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -3722,19 +3769,19 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B85" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C85" t="s">
         <v>133</v>
       </c>
       <c r="D85" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E85" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -3742,19 +3789,19 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B86" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="C86" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D86" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="E86" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -3762,19 +3809,19 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B87" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C87" t="s">
         <v>135</v>
       </c>
       <c r="D87" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="E87" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -3782,59 +3829,59 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>282</v>
+        <v>158</v>
       </c>
       <c r="B88" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C88" t="s">
         <v>135</v>
       </c>
       <c r="D88" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="E88" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F88">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>161</v>
+        <v>279</v>
       </c>
       <c r="B89" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C89" t="s">
         <v>135</v>
       </c>
       <c r="D89" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E89" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F89">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B90" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C90" t="s">
         <v>135</v>
       </c>
       <c r="D90" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="E90" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -3842,19 +3889,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B91" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C91" t="s">
         <v>135</v>
       </c>
       <c r="D91" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="E91" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -3862,59 +3909,59 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>283</v>
+        <v>165</v>
       </c>
       <c r="B92" t="s">
-        <v>142</v>
+        <v>166</v>
       </c>
       <c r="C92" t="s">
         <v>135</v>
       </c>
       <c r="D92" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="E92" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F92">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>167</v>
+        <v>280</v>
       </c>
       <c r="B93" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="C93" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D93" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
       <c r="E93" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F93">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C94" t="s">
         <v>133</v>
       </c>
       <c r="D94" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="E94" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -3922,19 +3969,19 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B95" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C95" t="s">
         <v>133</v>
       </c>
       <c r="D95" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="E95" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -3942,19 +3989,19 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B96" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C96" t="s">
         <v>133</v>
       </c>
       <c r="D96" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E96" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -3962,39 +4009,39 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>284</v>
+        <v>173</v>
       </c>
       <c r="B97" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C97" t="s">
         <v>133</v>
       </c>
       <c r="D97" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="E97" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F97">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B98" t="s">
-        <v>137</v>
+        <v>175</v>
       </c>
       <c r="C98" t="s">
         <v>133</v>
       </c>
       <c r="D98" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="E98" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F98">
         <v>2</v>
@@ -4002,19 +4049,19 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B99" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C99" t="s">
         <v>133</v>
       </c>
       <c r="D99" t="s">
-        <v>361</v>
+        <v>345</v>
       </c>
       <c r="E99" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F99">
         <v>2</v>
@@ -4022,139 +4069,139 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>176</v>
+        <v>283</v>
       </c>
       <c r="B100" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="C100" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D100" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="E100" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F100">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>287</v>
+        <v>176</v>
       </c>
       <c r="B101" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C101" t="s">
         <v>135</v>
       </c>
       <c r="D101" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="E101" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F101">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B102" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C102" t="s">
         <v>135</v>
       </c>
       <c r="D102" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E102" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F102">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>179</v>
+        <v>285</v>
       </c>
       <c r="B103" t="s">
-        <v>137</v>
+        <v>178</v>
       </c>
       <c r="C103" t="s">
         <v>135</v>
       </c>
       <c r="D103" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="E103" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F103">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>289</v>
+        <v>179</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C104" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D104" t="s">
-        <v>365</v>
+        <v>334</v>
       </c>
       <c r="E104" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F104">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>290</v>
+        <v>387</v>
       </c>
       <c r="B105" t="s">
-        <v>180</v>
+        <v>138</v>
       </c>
       <c r="C105" t="s">
         <v>133</v>
       </c>
       <c r="D105" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="E105" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F105">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>180</v>
+      </c>
+      <c r="B106" t="s">
         <v>181</v>
       </c>
-      <c r="B106" t="s">
+      <c r="C106" t="s">
         <v>182</v>
       </c>
-      <c r="C106" t="s">
-        <v>183</v>
-      </c>
       <c r="D106" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E106" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -4162,19 +4209,19 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
+        <v>183</v>
+      </c>
+      <c r="B107" t="s">
         <v>184</v>
       </c>
-      <c r="B107" t="s">
+      <c r="C107" t="s">
         <v>185</v>
       </c>
-      <c r="C107" t="s">
-        <v>186</v>
-      </c>
       <c r="D107" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="E107" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -4182,19 +4229,19 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B108" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D108" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="E108" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F108">
         <v>2</v>
@@ -4202,19 +4249,19 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B109" t="s">
+        <v>187</v>
+      </c>
+      <c r="C109" t="s">
         <v>188</v>
       </c>
-      <c r="C109" t="s">
-        <v>189</v>
-      </c>
       <c r="D109" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="E109" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F109">
         <v>2</v>
@@ -4222,19 +4269,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>189</v>
+      </c>
+      <c r="B110" t="s">
         <v>190</v>
       </c>
-      <c r="B110" t="s">
+      <c r="C110" t="s">
         <v>191</v>
       </c>
-      <c r="C110" t="s">
-        <v>192</v>
-      </c>
       <c r="D110" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="E110" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F110">
         <v>1</v>
@@ -4242,19 +4289,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
+        <v>192</v>
+      </c>
+      <c r="B111" t="s">
         <v>193</v>
       </c>
-      <c r="B111" t="s">
+      <c r="C111" t="s">
         <v>194</v>
       </c>
-      <c r="C111" t="s">
-        <v>195</v>
-      </c>
       <c r="D111" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="E111" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F111">
         <v>1</v>
@@ -4262,19 +4309,19 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
+        <v>195</v>
+      </c>
+      <c r="B112" t="s">
         <v>196</v>
       </c>
-      <c r="B112" t="s">
+      <c r="C112" t="s">
         <v>197</v>
       </c>
-      <c r="C112" t="s">
-        <v>198</v>
-      </c>
       <c r="D112" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="E112" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -4282,19 +4329,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B113" t="s">
+        <v>198</v>
+      </c>
+      <c r="C113" t="s">
         <v>199</v>
       </c>
-      <c r="C113" t="s">
-        <v>200</v>
-      </c>
       <c r="D113" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="E113" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F113">
         <v>9</v>
@@ -4302,19 +4349,19 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
+        <v>200</v>
+      </c>
+      <c r="B114" t="s">
         <v>201</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" t="s">
         <v>202</v>
       </c>
-      <c r="C114" t="s">
-        <v>203</v>
-      </c>
       <c r="D114" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="E114" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F114">
         <v>1</v>
@@ -4322,19 +4369,19 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
+        <v>203</v>
+      </c>
+      <c r="B115" t="s">
         <v>204</v>
       </c>
-      <c r="B115" t="s">
+      <c r="C115" t="s">
         <v>205</v>
       </c>
-      <c r="C115" t="s">
+      <c r="D115" t="s">
         <v>206</v>
       </c>
-      <c r="D115" t="s">
-        <v>207</v>
-      </c>
       <c r="E115" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -4342,19 +4389,19 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
+        <v>207</v>
+      </c>
+      <c r="B116" t="s">
         <v>208</v>
       </c>
-      <c r="B116" t="s">
+      <c r="C116" t="s">
         <v>209</v>
       </c>
-      <c r="C116" t="s">
-        <v>210</v>
-      </c>
       <c r="D116" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E116" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F116">
         <v>1</v>
@@ -4362,19 +4409,19 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="B117" t="s">
+        <v>210</v>
+      </c>
+      <c r="C117" t="s">
         <v>211</v>
       </c>
-      <c r="C117" t="s">
-        <v>212</v>
-      </c>
       <c r="D117" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E117" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F117">
         <v>2</v>
@@ -4382,19 +4429,19 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
+        <v>212</v>
+      </c>
+      <c r="B118" t="s">
         <v>213</v>
       </c>
-      <c r="B118" t="s">
+      <c r="C118" t="s">
         <v>214</v>
       </c>
-      <c r="C118" t="s">
-        <v>215</v>
-      </c>
       <c r="D118" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="E118" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F118">
         <v>1</v>
@@ -4402,19 +4449,19 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
+        <v>215</v>
+      </c>
+      <c r="B119" t="s">
         <v>216</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C119" t="s">
         <v>217</v>
       </c>
-      <c r="C119" t="s">
-        <v>218</v>
-      </c>
       <c r="D119" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="E119" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -4422,19 +4469,19 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
+        <v>218</v>
+      </c>
+      <c r="B120" t="s">
         <v>219</v>
       </c>
-      <c r="B120" t="s">
+      <c r="C120" t="s">
         <v>220</v>
       </c>
-      <c r="C120" t="s">
-        <v>221</v>
-      </c>
       <c r="D120" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="E120" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -4442,19 +4489,19 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
+        <v>221</v>
+      </c>
+      <c r="B121" t="s">
         <v>222</v>
       </c>
-      <c r="B121" t="s">
-        <v>223</v>
-      </c>
       <c r="C121" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D121" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="E121" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -4462,19 +4509,19 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
+        <v>223</v>
+      </c>
+      <c r="B122" t="s">
         <v>224</v>
       </c>
-      <c r="B122" t="s">
+      <c r="C122" t="s">
         <v>225</v>
       </c>
-      <c r="C122" t="s">
-        <v>226</v>
-      </c>
       <c r="D122" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="E122" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -4482,19 +4529,19 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
+        <v>226</v>
+      </c>
+      <c r="B123" t="s">
         <v>227</v>
-      </c>
-      <c r="B123" t="s">
-        <v>228</v>
       </c>
       <c r="C123" t="s">
         <v>85</v>
       </c>
       <c r="D123" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E123" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F123">
         <v>1</v>
@@ -4502,19 +4549,19 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
+        <v>228</v>
+      </c>
+      <c r="B124" t="s">
         <v>229</v>
       </c>
-      <c r="B124" t="s">
+      <c r="C124" t="s">
         <v>230</v>
       </c>
-      <c r="C124" t="s">
-        <v>231</v>
-      </c>
       <c r="D124" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E124" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -4522,19 +4569,19 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
+        <v>231</v>
+      </c>
+      <c r="B125" t="s">
         <v>232</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>233</v>
       </c>
-      <c r="C125" t="s">
-        <v>234</v>
-      </c>
       <c r="D125" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="E125" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -4542,19 +4589,19 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
+        <v>234</v>
+      </c>
+      <c r="B126" t="s">
         <v>235</v>
       </c>
-      <c r="B126" t="s">
+      <c r="C126" t="s">
         <v>236</v>
       </c>
-      <c r="C126" t="s">
-        <v>237</v>
-      </c>
       <c r="D126" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="E126" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F126">
         <v>1</v>
@@ -4562,19 +4609,19 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
+        <v>237</v>
+      </c>
+      <c r="B127" t="s">
         <v>238</v>
       </c>
-      <c r="B127" t="s">
+      <c r="C127" t="s">
         <v>239</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
         <v>240</v>
       </c>
-      <c r="D127" t="s">
-        <v>241</v>
-      </c>
       <c r="E127" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -4582,26 +4629,130 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B128" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C128" t="s">
+        <v>239</v>
+      </c>
+      <c r="D128" t="s">
         <v>240</v>
       </c>
-      <c r="D128" t="s">
-        <v>241</v>
-      </c>
       <c r="E128" t="s">
+        <v>376</v>
+      </c>
+      <c r="F128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>382</v>
+      </c>
+      <c r="B129" t="s">
         <v>383</v>
       </c>
-      <c r="F128">
+      <c r="C129" t="s">
+        <v>64</v>
+      </c>
+      <c r="D129" t="s">
+        <v>383</v>
+      </c>
+      <c r="E129" t="s">
+        <v>376</v>
+      </c>
+      <c r="F129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>384</v>
+      </c>
+      <c r="B130" t="s">
+        <v>137</v>
+      </c>
+      <c r="C130" t="s">
+        <v>135</v>
+      </c>
+      <c r="D130" t="s">
+        <v>334</v>
+      </c>
+      <c r="E130" t="s">
+        <v>376</v>
+      </c>
+      <c r="F130">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>385</v>
+      </c>
+      <c r="B131" t="s">
+        <v>136</v>
+      </c>
+      <c r="C131" t="s">
+        <v>135</v>
+      </c>
+      <c r="D131" t="s">
+        <v>333</v>
+      </c>
+      <c r="E131" t="s">
+        <v>376</v>
+      </c>
+      <c r="F131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>388</v>
+      </c>
+      <c r="B132" t="s">
+        <v>393</v>
+      </c>
+      <c r="C132" t="s">
+        <v>389</v>
+      </c>
+      <c r="D132" t="s">
+        <v>393</v>
+      </c>
+      <c r="E132" t="s">
+        <v>376</v>
+      </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>391</v>
+      </c>
+      <c r="B133" t="s">
+        <v>390</v>
+      </c>
+      <c r="C133" t="s">
+        <v>392</v>
+      </c>
+      <c r="D133" t="s">
+        <v>390</v>
+      </c>
+      <c r="E133" t="s">
+        <v>376</v>
+      </c>
+      <c r="F133">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D30" r:id="rId1" display="https://www.lcsc.com/product-detail/Crystals_TXC-Corp-7M25000013_C331585.html" xr:uid="{8EB884C0-EBEC-491A-B014-2392350C7772}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>